<commit_message>
overall changes in project
</commit_message>
<xml_diff>
--- a/RR/excel/GenericFlow/NewsFeedDelete.xlsx
+++ b/RR/excel/GenericFlow/NewsFeedDelete.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="572" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="580" uniqueCount="215">
   <si>
     <t>NewsFeed ID</t>
   </si>
@@ -664,6 +664,12 @@
   </si>
   <si>
     <t>4018904</t>
+  </si>
+  <si>
+    <t>4769416</t>
+  </si>
+  <si>
+    <t>4770267</t>
   </si>
 </sst>
 </file>
@@ -1015,7 +1021,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J209"/>
+  <dimension ref="A1:J213"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
       <selection activeCell="B56" sqref="B56"/>
@@ -2715,6 +2721,38 @@
         <v>59</v>
       </c>
     </row>
+    <row r="210">
+      <c r="A210" t="s">
+        <v>213</v>
+      </c>
+      <c r="B210" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="211">
+      <c r="A211" t="s">
+        <v>213</v>
+      </c>
+      <c r="B211" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="212">
+      <c r="A212" t="s">
+        <v>213</v>
+      </c>
+      <c r="B212" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="213">
+      <c r="A213" t="s">
+        <v>214</v>
+      </c>
+      <c r="B213" t="s">
+        <v>59</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="D1:J2"/>

</xml_diff>

<commit_message>
Cross browser and appreciate flow added
</commit_message>
<xml_diff>
--- a/RR/excel/GenericFlow/NewsFeedDelete.xlsx
+++ b/RR/excel/GenericFlow/NewsFeedDelete.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="234">
   <si>
     <t>NewsFeed ID</t>
   </si>
@@ -671,46 +671,64 @@
     <t>4920148</t>
   </si>
   <si>
+    <t>4920164</t>
+  </si>
+  <si>
+    <t>4920193</t>
+  </si>
+  <si>
+    <t>4920209</t>
+  </si>
+  <si>
+    <t>4920234</t>
+  </si>
+  <si>
+    <t>4922293</t>
+  </si>
+  <si>
+    <t>4922332</t>
+  </si>
+  <si>
+    <t>4923435</t>
+  </si>
+  <si>
+    <t>4923837</t>
+  </si>
+  <si>
+    <t>4929617</t>
+  </si>
+  <si>
+    <t>5039055</t>
+  </si>
+  <si>
+    <t>5039091</t>
+  </si>
+  <si>
+    <t>5039165</t>
+  </si>
+  <si>
+    <t>5039208</t>
+  </si>
+  <si>
+    <t>5066292</t>
+  </si>
+  <si>
+    <t>5066298</t>
+  </si>
+  <si>
     <t>Pending</t>
   </si>
   <si>
-    <t>4920164</t>
-  </si>
-  <si>
-    <t>4920193</t>
-  </si>
-  <si>
-    <t>4920209</t>
-  </si>
-  <si>
-    <t>4920234</t>
-  </si>
-  <si>
-    <t>4922293</t>
-  </si>
-  <si>
-    <t>4922332</t>
-  </si>
-  <si>
-    <t>4923435</t>
-  </si>
-  <si>
-    <t>4923837</t>
-  </si>
-  <si>
-    <t>4929617</t>
-  </si>
-  <si>
-    <t>5039055</t>
-  </si>
-  <si>
-    <t>5039091</t>
-  </si>
-  <si>
-    <t>5039165</t>
-  </si>
-  <si>
-    <t>5039208</t>
+    <t>5066305</t>
+  </si>
+  <si>
+    <t>5066326</t>
+  </si>
+  <si>
+    <t>5066445</t>
+  </si>
+  <si>
+    <t>5070617</t>
   </si>
 </sst>
 </file>
@@ -1672,10 +1690,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:J228"/>
+  <dimension ref="A1:J234"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A204" workbookViewId="0">
-      <selection activeCell="D218" sqref="D218"/>
+    <sheetView tabSelected="1" topLeftCell="A219" workbookViewId="0">
+      <selection activeCell="B232" sqref="B232"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -3414,7 +3432,7 @@
     </row>
     <row r="215" spans="1:2">
       <c r="A215" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B215" t="s">
         <v>4</v>
@@ -3422,7 +3440,7 @@
     </row>
     <row r="216" spans="1:2">
       <c r="A216" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B216" t="s">
         <v>4</v>
@@ -3430,7 +3448,7 @@
     </row>
     <row r="217" spans="1:2">
       <c r="A217" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B217" t="s">
         <v>4</v>
@@ -3438,90 +3456,138 @@
     </row>
     <row r="218" spans="1:2">
       <c r="A218" t="s">
+        <v>217</v>
+      </c>
+      <c r="B218" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="219" spans="1:2">
+      <c r="A219" t="s">
         <v>218</v>
       </c>
-      <c r="B218" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="219">
-      <c r="A219" t="s">
+      <c r="B219" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="220" spans="1:2">
+      <c r="A220" t="s">
         <v>219</v>
       </c>
-      <c r="B219" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="220">
-      <c r="A220" t="s">
+      <c r="B220" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="221" spans="1:2">
+      <c r="A221" t="s">
+        <v>219</v>
+      </c>
+      <c r="B221" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="222" spans="1:2">
+      <c r="A222" t="s">
         <v>220</v>
       </c>
-      <c r="B220" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="221">
-      <c r="A221" t="s">
-        <v>220</v>
-      </c>
-      <c r="B221" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="222">
-      <c r="A222" t="s">
+      <c r="B222" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="223" spans="1:2">
+      <c r="A223" t="s">
         <v>221</v>
       </c>
-      <c r="B222" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="223">
-      <c r="A223" t="s">
+      <c r="B223" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="224" spans="1:2">
+      <c r="A224" t="s">
         <v>222</v>
       </c>
-      <c r="B223" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="224">
-      <c r="A224" t="s">
+      <c r="B224" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="225" spans="1:2">
+      <c r="A225" t="s">
         <v>223</v>
       </c>
-      <c r="B224" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="225">
-      <c r="A225" t="s">
+      <c r="B225" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="226" spans="1:2">
+      <c r="A226" t="s">
         <v>224</v>
       </c>
-      <c r="B225" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="226">
-      <c r="A226" t="s">
+      <c r="B226" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="227" spans="1:2">
+      <c r="A227" t="s">
         <v>225</v>
       </c>
-      <c r="B226" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="227">
-      <c r="A227" t="s">
+      <c r="B227" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="228" spans="1:2">
+      <c r="A228" t="s">
         <v>226</v>
       </c>
-      <c r="B227" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="228">
-      <c r="A228" t="s">
+      <c r="B228" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="229" spans="1:2">
+      <c r="A229" t="s">
         <v>227</v>
       </c>
-      <c r="B228" t="s">
-        <v>4</v>
+      <c r="B229" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="230" spans="1:2">
+      <c r="A230" t="s">
+        <v>228</v>
+      </c>
+      <c r="B230" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="231" spans="1:2">
+      <c r="A231" t="s">
+        <v>230</v>
+      </c>
+      <c r="B231" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="232" spans="1:2">
+      <c r="A232" t="s">
+        <v>231</v>
+      </c>
+      <c r="B232" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="233">
+      <c r="A233" t="s">
+        <v>232</v>
+      </c>
+      <c r="B233" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="234">
+      <c r="A234" t="s">
+        <v>233</v>
+      </c>
+      <c r="B234" t="s">
+        <v>229</v>
       </c>
     </row>
   </sheetData>

</xml_diff>